<commit_message>
Adding questions for 2 feb 11 am
</commit_message>
<xml_diff>
--- a/asp1feb9pm.xlsx
+++ b/asp1feb9pm.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT cell\Desktop\papers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT cell\PycharmProjects\TestSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADB5C19-8A29-44D3-BD0D-BDC931D67EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969B9DC8-62FD-48BE-8A6B-6BEA51F9A62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8CB73E9A-CD66-4193-98AC-ACECBF6BFCBC}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="392">
-  <si>
-    <t>B</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="388">
   <si>
     <t>None of the above.</t>
   </si>
@@ -45,9 +42,6 @@
     <t xml:space="preserve"> What is the use of VaryByParam attribute in OutputCache directive?</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>Use the AutoDetect setting of the cookieless attribute.</t>
   </si>
   <si>
@@ -58,9 +52,6 @@
   </si>
   <si>
     <t xml:space="preserve"> If any user has disabled cookies in their browsers, what can you do to enable them to use forms authentication?</t>
-  </si>
-  <si>
-    <t>A</t>
   </si>
   <si>
     <t>In the authorization section of the Machine.config file, set the users attribute to the allow element to “?”.</t>
@@ -203,9 +194,6 @@
 Statement 2: Authorization is the process of determining whether a user is permitted to access to any part of an application, or any particular resource. 
 Statement 3: Authorization is the process that determines the identity of a user. 
 Statement 4: Authentication is the process of determining whether a user is permitted access to any part of an application, or any particular resource.</t>
-  </si>
-  <si>
-    <t>D</t>
   </si>
   <si>
     <t>All of the above</t>
@@ -1582,7 +1570,7 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,25 +1585,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D1" t="s">
+        <v>384</v>
+      </c>
+      <c r="E1" t="s">
         <v>385</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>386</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>387</v>
-      </c>
-      <c r="D1" t="s">
-        <v>388</v>
-      </c>
-      <c r="E1" t="s">
-        <v>389</v>
-      </c>
-      <c r="F1" t="s">
-        <v>390</v>
-      </c>
-      <c r="G1" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1623,22 +1611,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>57</v>
+        <v>171</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1646,22 +1634,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1669,22 +1657,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1692,22 +1680,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>372</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1715,22 +1703,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>44</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1738,22 +1726,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>57</v>
+        <v>368</v>
+      </c>
+      <c r="G7" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1761,22 +1749,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>6</v>
+        <v>365</v>
+      </c>
+      <c r="G8" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1784,22 +1772,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>11</v>
+        <v>363</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -1807,22 +1795,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1830,22 +1818,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -1853,22 +1841,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1876,22 +1864,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>0</v>
+        <v>353</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1899,22 +1887,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>11</v>
+        <v>348</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1922,22 +1910,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>11</v>
+        <v>114</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1945,22 +1933,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>6</v>
+        <v>87</v>
+      </c>
+      <c r="G16" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1968,22 +1956,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1991,22 +1979,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>11</v>
+        <v>334</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2014,22 +2002,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2037,22 +2025,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>0</v>
+        <v>328</v>
+      </c>
+      <c r="G20" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2060,22 +2048,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>57</v>
+        <v>187</v>
+      </c>
+      <c r="G21" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2083,22 +2071,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>0</v>
+        <v>319</v>
+      </c>
+      <c r="G22" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2106,22 +2094,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>0</v>
+        <v>314</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2129,22 +2117,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
         <v>1</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2152,22 +2140,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2175,22 +2163,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>0</v>
+        <v>304</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2198,22 +2186,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="G27" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2221,22 +2209,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>6</v>
+        <v>298</v>
+      </c>
+      <c r="G28" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2244,22 +2232,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -2267,22 +2255,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2290,22 +2278,22 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G31" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2313,22 +2301,22 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G32" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2336,22 +2324,22 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>57</v>
+        <v>285</v>
+      </c>
+      <c r="G33" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2359,22 +2347,22 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="G34" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2382,22 +2370,22 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>57</v>
+        <v>281</v>
+      </c>
+      <c r="G35" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2405,22 +2393,22 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>0</v>
+        <v>114</v>
+      </c>
+      <c r="G36" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2428,22 +2416,22 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>6</v>
+        <v>114</v>
+      </c>
+      <c r="G37" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2451,22 +2439,22 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="G38" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2474,22 +2462,22 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1">
         <v>1</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -2497,22 +2485,22 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G40" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="G40" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -2520,22 +2508,22 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
+      </c>
+      <c r="G41" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2543,22 +2531,22 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>11</v>
+        <v>257</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2566,22 +2554,22 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>57</v>
+        <v>134</v>
+      </c>
+      <c r="G43" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2589,22 +2577,22 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>0</v>
+        <v>248</v>
+      </c>
+      <c r="G44" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2612,22 +2600,22 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>57</v>
+        <v>243</v>
+      </c>
+      <c r="G45" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2635,22 +2623,22 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>0</v>
+        <v>238</v>
+      </c>
+      <c r="G46" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2658,22 +2646,22 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>57</v>
+        <v>233</v>
+      </c>
+      <c r="G47" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2681,22 +2669,22 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>0</v>
+        <v>228</v>
+      </c>
+      <c r="G48" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2704,22 +2692,22 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
+      </c>
+      <c r="G49" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2727,22 +2715,22 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>57</v>
+        <v>221</v>
+      </c>
+      <c r="G50" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2750,22 +2738,22 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="G51" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2773,22 +2761,22 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>6</v>
+        <v>214</v>
+      </c>
+      <c r="G52" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2796,22 +2784,22 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>11</v>
+        <v>209</v>
+      </c>
+      <c r="G53" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2819,22 +2807,22 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>11</v>
+        <v>204</v>
+      </c>
+      <c r="G54" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2842,22 +2830,22 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>57</v>
+        <v>199</v>
+      </c>
+      <c r="G55" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2865,22 +2853,22 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G56" s="1">
         <v>1</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:7" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -2888,22 +2876,22 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="G57" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:7" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -2911,22 +2899,22 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="G58" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:7" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -2934,22 +2922,22 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>6</v>
+        <v>182</v>
+      </c>
+      <c r="G59" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2957,22 +2945,22 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>6</v>
+        <v>87</v>
+      </c>
+      <c r="G60" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2980,22 +2968,22 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>11</v>
+        <v>114</v>
+      </c>
+      <c r="G61" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3003,22 +2991,22 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>57</v>
+        <v>171</v>
+      </c>
+      <c r="G62" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3026,22 +3014,22 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>57</v>
+        <v>166</v>
+      </c>
+      <c r="G63" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:7" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -3049,22 +3037,22 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
+      </c>
+      <c r="G64" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:7" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -3072,22 +3060,22 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G65" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="G65" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3095,22 +3083,22 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
+      </c>
+      <c r="G66" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3118,22 +3106,22 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>57</v>
+        <v>149</v>
+      </c>
+      <c r="G67" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3141,22 +3129,22 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>11</v>
+        <v>144</v>
+      </c>
+      <c r="G68" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -3164,22 +3152,22 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G69" s="1">
         <v>1</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3187,22 +3175,22 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G70" s="1">
         <v>1</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="71" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3210,22 +3198,22 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>11</v>
+        <v>131</v>
+      </c>
+      <c r="G71" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3233,22 +3221,22 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="G72" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3256,22 +3244,22 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
+      </c>
+      <c r="G73" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3279,22 +3267,22 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+      <c r="G74" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3302,22 +3290,22 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>0</v>
+        <v>114</v>
+      </c>
+      <c r="G75" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3325,22 +3313,22 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>6</v>
+        <v>109</v>
+      </c>
+      <c r="G76" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3348,22 +3336,22 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="G77" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:7" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -3371,22 +3359,22 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1">
         <v>1</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="79" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3394,22 +3382,22 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>6</v>
+        <v>96</v>
+      </c>
+      <c r="G79" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3417,22 +3405,22 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>11</v>
+        <v>91</v>
+      </c>
+      <c r="G80" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3440,22 +3428,22 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>57</v>
+        <v>86</v>
+      </c>
+      <c r="G81" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3463,7 +3451,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C82" s="1">
         <v>70</v>
@@ -3477,8 +3465,8 @@
       <c r="F82" s="1">
         <v>410</v>
       </c>
-      <c r="G82" s="1" t="s">
-        <v>0</v>
+      <c r="G82" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3486,22 +3474,22 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G83" s="1">
         <v>1</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3509,22 +3497,22 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="G84" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3532,22 +3520,22 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G85" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="G85" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -3555,22 +3543,22 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
+      </c>
+      <c r="G86" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:7" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -3578,22 +3566,22 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>11</v>
+        <v>63</v>
+      </c>
+      <c r="G87" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -3601,22 +3589,22 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G88" s="1">
         <v>1</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3624,22 +3612,22 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="G89" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:7" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -3647,22 +3635,22 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>11</v>
+        <v>49</v>
+      </c>
+      <c r="G90" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -3670,22 +3658,22 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>11</v>
+        <v>44</v>
+      </c>
+      <c r="G91" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -3693,22 +3681,22 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G92" s="1">
         <v>1</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="93" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3716,22 +3704,22 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
+      </c>
+      <c r="G93" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3739,22 +3727,22 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
+      </c>
+      <c r="G94" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3762,22 +3750,22 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G95" s="1">
         <v>1</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:7" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -3785,22 +3773,22 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G96" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="G96" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:7" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -3808,22 +3796,22 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="G97" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3831,22 +3819,22 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G98" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="G98" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:7" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -3854,22 +3842,22 @@
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G99" s="1">
         <v>1</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="100" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -3877,22 +3865,22 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="G100" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:7" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -3900,22 +3888,22 @@
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E101" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G101" s="1">
         <v>2</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>